<commit_message>
update sclaing factors of aCCFs, modify names of settings, and seprating configuration file from main script and including it in yml file
</commit_message>
<xml_diff>
--- a/build/lib/envlib/database/Mission_EINOx_AC_v2.xlsx
+++ b/build/lib/envlib/database/Mission_EINOx_AC_v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abolfazlsimorgh/Documents/SEsarProject/ALARM/envlib/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abolfazlsimorgh/Documents/CLIMaCCF/envlib/envlib/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ECDAB6-1111-7546-A079-C0F9C1206032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7151CFF-AEA2-E941-90C6-3EBD6374D16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22300" windowHeight="13860" xr2:uid="{0C110B6A-D4FB-47C3-84FA-8BDBA3E6D7D0}"/>
   </bookViews>
@@ -29,28 +29,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>EI inverse range [km/kg] wide-body</t>
-  </si>
-  <si>
-    <t>EI inverse range [km/kg] single-aisle</t>
-  </si>
-  <si>
-    <t>EI inverse range [km/kg] regional</t>
-  </si>
-  <si>
     <t>altitude [ft]</t>
   </si>
   <si>
-    <t>EI NOx regional [g/kg Fuel]</t>
+    <t>pressure level [hPa]</t>
   </si>
   <si>
-    <t>EI NOx single-aisle [g/kg Fuel]</t>
+    <t>EI NOx regional [g/kg(Fuel)]</t>
   </si>
   <si>
-    <t>EI NOx wide-body [g/kg Fuel]</t>
+    <t>EI NOx single-aisle [g/kg(Fuel)]</t>
   </si>
   <si>
-    <t>pressure level [hPa]</t>
+    <t>EI NOx wide-body [g/kg(Fuel)]</t>
+  </si>
+  <si>
+    <t>flown distance [km/kg(fuel)] regional</t>
+  </si>
+  <si>
+    <t>flown distance [km/kg(fuel)] single-aisle</t>
+  </si>
+  <si>
+    <t>flown distance [km/kg(fuel)] wide-body</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:A29"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -422,28 +422,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>